<commit_message>
final k vs acc results
</commit_message>
<xml_diff>
--- a/results/k vs acc/k vs acc.xlsx
+++ b/results/k vs acc/k vs acc.xlsx
@@ -1,41 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kuba\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ewolucja\ewolucja_sieci\results\k vs acc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15FC005-1535-406B-AF31-5104839105CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>k</t>
   </si>
   <si>
     <t>acc</t>
   </si>
+  <si>
+    <t>std</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,7 +101,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
   <c:roundedCorners val="0"/>
@@ -130,7 +145,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -253,6 +267,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD4F-4C5E-8B40-30C655FD1153}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -318,7 +337,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -441,7 +459,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1117,20 +1134,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>213359</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>403858</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvPr id="2" name="Wykres 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1410,32 +1433,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D10" sqref="C10:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
         <v>88.58</v>
       </c>
+      <c r="C2">
+        <f>STDEVPA(B2:B6)</f>
+        <v>3.2804121692250821</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1443,7 +1476,7 @@
         <v>88.14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1451,7 +1484,7 @@
         <v>87.64</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1459,7 +1492,7 @@
         <v>82.35</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>

</xml_diff>